<commit_message>
testing of KMeans is done and is under results folder
</commit_message>
<xml_diff>
--- a/results/KMeans_Result.xlsx
+++ b/results/KMeans_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\OneDrive\Desktop\Rust-Projects\ML_ALGO_Rewite\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04201BEA-F172-4FEB-A0DE-7A1FA53B7C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D8BC69-89DA-4D26-ABA4-99B4C7F7A6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5160695A-4EBD-48E9-9256-CB4BF757272C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>DATASET</t>
   </si>
@@ -82,6 +82,75 @@
   </si>
   <si>
     <t>0.000338 s</t>
+  </si>
+  <si>
+    <t>Sample Hack Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.068482 s</t>
+  </si>
+  <si>
+    <t>0.001121 s</t>
+  </si>
+  <si>
+    <t>0.069484 s</t>
+  </si>
+  <si>
+    <t>0.000955 s</t>
+  </si>
+  <si>
+    <t>0.000945 s</t>
+  </si>
+  <si>
+    <t>0.065585 s</t>
+  </si>
+  <si>
+    <t>0.000213 s</t>
+  </si>
+  <si>
+    <t>0.075676 s</t>
+  </si>
+  <si>
+    <t>Credit Card Customer Data</t>
+  </si>
+  <si>
+    <t>student_performance</t>
+  </si>
+  <si>
+    <t>Mall_Customers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22.145ms</t>
+  </si>
+  <si>
+    <t>3.3849ms</t>
+  </si>
+  <si>
+    <t>49.3692ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.5976ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> skipped (dataset too large: 14003 samples)</t>
+  </si>
+  <si>
+    <t>672.6516ms</t>
+  </si>
+  <si>
+    <t>73.075ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.5642ms</t>
+  </si>
+  <si>
+    <t>894.5µs</t>
+  </si>
+  <si>
+    <t>33.0354ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6.7235ms</t>
   </si>
 </sst>
 </file>
@@ -433,19 +502,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C86715F-181E-491A-9DAE-938C5D4669F4}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="41" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" customWidth="1"/>
     <col min="8" max="8" width="28.42578125" customWidth="1"/>
@@ -504,20 +573,202 @@
       <c r="B2">
         <v>36528388099.321999</v>
       </c>
+      <c r="C2">
+        <v>36528388099.321999</v>
+      </c>
       <c r="D2">
         <v>0.72563148587909398</v>
       </c>
+      <c r="E2">
+        <v>0.72563148587909398</v>
+      </c>
       <c r="F2">
         <v>0.51903079486517401</v>
       </c>
+      <c r="G2">
+        <v>0.519030794865175</v>
+      </c>
       <c r="H2">
         <v>365.569495897016</v>
       </c>
+      <c r="I2">
+        <v>365.569495897016</v>
+      </c>
       <c r="J2" t="s">
         <v>14</v>
       </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
       <c r="L2" t="s">
         <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>748453645657.82495</v>
+      </c>
+      <c r="C3">
+        <v>760529014052.61694</v>
+      </c>
+      <c r="D3">
+        <v>0.62962938004549396</v>
+      </c>
+      <c r="E3">
+        <v>0.50080512590602899</v>
+      </c>
+      <c r="F3">
+        <v>0.62556195507549295</v>
+      </c>
+      <c r="G3">
+        <v>0.92850522883973197</v>
+      </c>
+      <c r="H3">
+        <v>542.71569921305399</v>
+      </c>
+      <c r="I3">
+        <v>523.65122680305899</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>7166053.9505460002</v>
+      </c>
+      <c r="C4">
+        <v>7166058.8818704505</v>
+      </c>
+      <c r="D4">
+        <v>0.27627451802386799</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>1.42521565904897</v>
+      </c>
+      <c r="G4">
+        <v>1.42521377459166</v>
+      </c>
+      <c r="H4">
+        <v>6464.3486941232604</v>
+      </c>
+      <c r="I4">
+        <v>6464.3346108914302</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>387114.74027399998</v>
+      </c>
+      <c r="C5">
+        <v>387114.74027402699</v>
+      </c>
+      <c r="D5">
+        <v>0.47926366436618301</v>
+      </c>
+      <c r="E5">
+        <v>0.47926366436618401</v>
+      </c>
+      <c r="F5">
+        <v>0.76591411115234498</v>
+      </c>
+      <c r="G5">
+        <v>0.76591411115234498</v>
+      </c>
+      <c r="H5">
+        <v>300.97646672732401</v>
+      </c>
+      <c r="I5">
+        <v>300.97646672732401</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>6915190.6272700001</v>
+      </c>
+      <c r="C6">
+        <v>6915190.6272704499</v>
+      </c>
+      <c r="D6">
+        <v>0.64161761953179597</v>
+      </c>
+      <c r="E6">
+        <v>0.64161761953179497</v>
+      </c>
+      <c r="F6">
+        <v>0.46420287440166702</v>
+      </c>
+      <c r="G6">
+        <v>0.46420287440162999</v>
+      </c>
+      <c r="H6">
+        <v>985.08343154885495</v>
+      </c>
+      <c r="I6">
+        <v>985.08343154885597</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>